<commit_message>
Added new style for report
</commit_message>
<xml_diff>
--- a/reports/report_20250604_20250605.xlsx
+++ b/reports/report_20250604_20250605.xlsx
@@ -29,12 +29,18 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFD966"/>
+        <bgColor rgb="00FFD966"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,9 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -425,97 +434,99 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="29" customWidth="1" min="3" max="3"/>
+    <col width="6" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>table_id</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>waiter</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>foods</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>sum</t>
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Номер стола</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Официант</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Заказ</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Чек</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" t="n">
         <v>8</v>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Vector</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Vector</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
           <t>Sprite 2л</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="D2" t="n">
         <v>1000</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B3" t="n">
+      <c r="A3" t="n">
         <v>8</v>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Vector</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Vector</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
           <t>Sprite 2л</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="D3" t="n">
         <v>1000</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B4" t="n">
+      <c r="A4" t="n">
         <v>9</v>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Eрарыс</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Eрарыс</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
           <t>Шашлык Баранина - Sprite 2л</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="D4" t="n">
         <v>2900</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" t="n">
+        <v>4900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>